<commit_message>
add site review video
</commit_message>
<xml_diff>
--- a/CinemeOnlineWeb/testSite.xlsx
+++ b/CinemeOnlineWeb/testSite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA64C7E-1D80-4E5B-852C-BBDAC7C032D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5293CDC7-8519-462C-B632-822E4B63B736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2412" yWindow="1128" windowWidth="17280" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testSite" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>James</t>
   </si>
   <si>
-    <t>COP CAR 2</t>
+    <t>COP 2</t>
   </si>
   <si>
-    <t>COP CAR</t>
+    <t>Hames</t>
+  </si>
+  <si>
+    <t>Jake</t>
+  </si>
+  <si>
+    <t>COPP</t>
   </si>
 </sst>
 </file>
@@ -887,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -903,7 +909,7 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>1900</v>
       </c>
       <c r="C1">
         <v>2</v>
@@ -917,24 +923,33 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2">
+        <v>2000</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1900</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
         <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>